<commit_message>
commit quy phong thang 10
</commit_message>
<xml_diff>
--- a/Quy Phong.xlsx
+++ b/Quy Phong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="298">
   <si>
     <t>Thang 01/2012</t>
   </si>
@@ -808,40 +808,7 @@
     <t>Quy Thang 08/2015</t>
   </si>
   <si>
-    <t>Clear Bac ha</t>
-  </si>
-  <si>
-    <t>Clear Men</t>
-  </si>
-  <si>
-    <t>H&amp;S Bac Ha</t>
-  </si>
-  <si>
     <t>Tien sieu thi</t>
-  </si>
-  <si>
-    <t>Safe guard</t>
-  </si>
-  <si>
-    <t>Kiwi</t>
-  </si>
-  <si>
-    <t>axe</t>
-  </si>
-  <si>
-    <t>Baguette</t>
-  </si>
-  <si>
-    <t>Dui ga</t>
-  </si>
-  <si>
-    <t>Nutri</t>
-  </si>
-  <si>
-    <t>Vina cafe</t>
-  </si>
-  <si>
-    <t>Comfor</t>
   </si>
   <si>
     <t>lau</t>
@@ -953,13 +920,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0_);_(\$* \(#,##0\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1114,7 +1080,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1216,10 +1182,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1346,8 +1308,8 @@
   </sheetPr>
   <dimension ref="A5:Q65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A375" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D385" activeCellId="0" sqref="D385"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F372" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I386" activeCellId="0" sqref="I386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9710,6 +9672,13 @@
       <c r="C379" s="17"/>
       <c r="D379" s="17"/>
       <c r="E379" s="17"/>
+      <c r="H379" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="I379" s="17"/>
+      <c r="J379" s="17"/>
+      <c r="K379" s="17"/>
+      <c r="L379" s="17"/>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
@@ -9727,14 +9696,20 @@
       <c r="E380" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I380" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="J380" s="25" t="n">
-        <v>77000</v>
-      </c>
-      <c r="K380" s="0" t="s">
-        <v>19</v>
+      <c r="H380" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I380" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J380" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K380" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L380" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9751,14 +9726,18 @@
       <c r="E381" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I381" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="J381" s="25" t="n">
-        <v>87500</v>
-      </c>
-      <c r="K381" s="0" t="s">
-        <v>239</v>
+      <c r="H381" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I381" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J381" s="23"/>
+      <c r="K381" s="4" t="n">
+        <v>163000</v>
+      </c>
+      <c r="L381" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9776,15 +9755,19 @@
       <c r="E382" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I382" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J382" s="25" t="n">
-        <f aca="false">26500*2</f>
-        <v>53000</v>
-      </c>
-      <c r="K382" s="0" t="s">
-        <v>42</v>
+      <c r="H382" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I382" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J382" s="23"/>
+      <c r="K382" s="4" t="n">
+        <f aca="false">800000*5</f>
+        <v>4000000</v>
+      </c>
+      <c r="L382" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9801,14 +9784,18 @@
       <c r="E383" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I383" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="J383" s="25" t="n">
-        <v>82000</v>
-      </c>
-      <c r="K383" s="0" t="s">
-        <v>211</v>
+      <c r="H383" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I383" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J383" s="23"/>
+      <c r="K383" s="4" t="n">
+        <v>3900000</v>
+      </c>
+      <c r="L383" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9823,17 +9810,20 @@
         <v>307000</v>
       </c>
       <c r="E384" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="I384" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="J384" s="25" t="n">
-        <f aca="false">10400*2</f>
-        <v>20800</v>
-      </c>
-      <c r="K384" s="0" t="s">
-        <v>19</v>
+        <v>262</v>
+      </c>
+      <c r="H384" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="I384" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J384" s="4"/>
+      <c r="K384" s="4" t="n">
+        <v>104000</v>
+      </c>
+      <c r="L384" s="4" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9844,14 +9834,18 @@
       <c r="C385" s="23"/>
       <c r="D385" s="4"/>
       <c r="E385" s="4"/>
-      <c r="I385" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="J385" s="25" t="n">
-        <v>53000</v>
-      </c>
-      <c r="K385" s="0" t="s">
-        <v>19</v>
+      <c r="H385" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="I385" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J385" s="23"/>
+      <c r="K385" s="4" t="n">
+        <v>34000</v>
+      </c>
+      <c r="L385" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9862,15 +9856,13 @@
       <c r="C386" s="4"/>
       <c r="D386" s="4"/>
       <c r="E386" s="4"/>
-      <c r="I386" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="J386" s="25" t="n">
-        <v>94100</v>
-      </c>
-      <c r="K386" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="H386" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I386" s="4"/>
+      <c r="J386" s="4"/>
+      <c r="K386" s="4"/>
+      <c r="L386" s="4"/>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="19" t="n">
@@ -9880,15 +9872,13 @@
       <c r="C387" s="24"/>
       <c r="D387" s="4"/>
       <c r="E387" s="4"/>
-      <c r="I387" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="J387" s="25" t="n">
-        <v>4500</v>
-      </c>
-      <c r="K387" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="H387" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="I387" s="4"/>
+      <c r="J387" s="24"/>
+      <c r="K387" s="4"/>
+      <c r="L387" s="4"/>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="19" t="n">
@@ -9898,15 +9888,13 @@
       <c r="C388" s="24"/>
       <c r="D388" s="4"/>
       <c r="E388" s="4"/>
-      <c r="I388" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="J388" s="25" t="n">
-        <v>13600</v>
-      </c>
-      <c r="K388" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="H388" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="I388" s="4"/>
+      <c r="J388" s="24"/>
+      <c r="K388" s="4"/>
+      <c r="L388" s="4"/>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="18" t="n">
@@ -9916,15 +9904,13 @@
       <c r="C389" s="23"/>
       <c r="D389" s="4"/>
       <c r="E389" s="4"/>
-      <c r="I389" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="J389" s="25" t="n">
-        <v>10200</v>
-      </c>
-      <c r="K389" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="H389" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I389" s="4"/>
+      <c r="J389" s="23"/>
+      <c r="K389" s="4"/>
+      <c r="L389" s="4"/>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="18" t="n">
@@ -9934,15 +9920,13 @@
       <c r="C390" s="23"/>
       <c r="D390" s="4"/>
       <c r="E390" s="4"/>
-      <c r="I390" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="J390" s="25" t="n">
-        <v>63900</v>
-      </c>
-      <c r="K390" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="H390" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="I390" s="4"/>
+      <c r="J390" s="23"/>
+      <c r="K390" s="4"/>
+      <c r="L390" s="4"/>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="18" t="n">
@@ -9952,15 +9936,13 @@
       <c r="C391" s="23"/>
       <c r="D391" s="4"/>
       <c r="E391" s="4"/>
-      <c r="I391" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="J391" s="25" t="n">
-        <v>94600</v>
-      </c>
-      <c r="K391" s="0" t="s">
-        <v>42</v>
-      </c>
+      <c r="H391" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="I391" s="4"/>
+      <c r="J391" s="23"/>
+      <c r="K391" s="4"/>
+      <c r="L391" s="4"/>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="18" t="n">
@@ -9970,15 +9952,13 @@
       <c r="C392" s="23"/>
       <c r="D392" s="4"/>
       <c r="E392" s="4"/>
-      <c r="I392" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="J392" s="25" t="n">
-        <v>159000</v>
-      </c>
-      <c r="K392" s="0" t="s">
-        <v>42</v>
-      </c>
+      <c r="H392" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="I392" s="4"/>
+      <c r="J392" s="23"/>
+      <c r="K392" s="4"/>
+      <c r="L392" s="4"/>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="18" t="n">
@@ -9988,6 +9968,13 @@
       <c r="C393" s="23"/>
       <c r="D393" s="4"/>
       <c r="E393" s="4"/>
+      <c r="H393" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="I393" s="4"/>
+      <c r="J393" s="23"/>
+      <c r="K393" s="4"/>
+      <c r="L393" s="4"/>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="18" t="n">
@@ -9997,6 +9984,13 @@
       <c r="C394" s="23"/>
       <c r="D394" s="4"/>
       <c r="E394" s="4"/>
+      <c r="H394" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="I394" s="4"/>
+      <c r="J394" s="23"/>
+      <c r="K394" s="4"/>
+      <c r="L394" s="4"/>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="18" t="n">
@@ -10006,13 +10000,13 @@
       <c r="C395" s="23"/>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
-      <c r="I395" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J395" s="25" t="n">
-        <f aca="false">SUMIF($K$380:$K$392,I395,$J$380:$J$392)</f>
-        <v>337100</v>
-      </c>
+      <c r="H395" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="I395" s="4"/>
+      <c r="J395" s="23"/>
+      <c r="K395" s="4"/>
+      <c r="L395" s="4"/>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="18" t="n">
@@ -10022,16 +10016,13 @@
       <c r="C396" s="23"/>
       <c r="D396" s="4"/>
       <c r="E396" s="4"/>
-      <c r="I396" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="J396" s="25" t="n">
-        <f aca="false">SUMIF($K$380:$K$392,I396,$J$380:$J$392)</f>
-        <v>87500</v>
-      </c>
-      <c r="K396" s="0" t="n">
-        <v>18000</v>
-      </c>
+      <c r="H396" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="I396" s="4"/>
+      <c r="J396" s="23"/>
+      <c r="K396" s="4"/>
+      <c r="L396" s="4"/>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
@@ -10044,13 +10035,16 @@
         <v>4404000</v>
       </c>
       <c r="E397" s="4"/>
-      <c r="I397" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J397" s="25" t="n">
-        <f aca="false">SUMIF($K$380:$K$392,I397,$J$380:$J$392)</f>
-        <v>306600</v>
-      </c>
+      <c r="H397" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I397" s="2"/>
+      <c r="J397" s="2"/>
+      <c r="K397" s="4" t="n">
+        <f aca="false">SUMIF(I381:I396,"T",K381:K396)</f>
+        <v>4163000</v>
+      </c>
+      <c r="L397" s="4"/>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
@@ -10063,16 +10057,16 @@
         <v>4241000</v>
       </c>
       <c r="E398" s="4"/>
-      <c r="I398" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="J398" s="25" t="n">
-        <f aca="false">SUMIF($K$380:$K$392,I398,$J$380:$J$392)</f>
-        <v>82000</v>
-      </c>
-      <c r="K398" s="0" t="n">
-        <v>9000</v>
-      </c>
+      <c r="H398" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I398" s="2"/>
+      <c r="J398" s="2"/>
+      <c r="K398" s="4" t="n">
+        <f aca="false">SUMIF(I381:I396,"C",K381:K396)</f>
+        <v>4038000</v>
+      </c>
+      <c r="L398" s="4"/>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
@@ -10085,14 +10079,16 @@
         <v>163000</v>
       </c>
       <c r="E399" s="4"/>
-      <c r="J399" s="25" t="n">
-        <f aca="false">SUM(J395:J398)</f>
-        <v>813200</v>
-      </c>
-      <c r="K399" s="25" t="n">
-        <f aca="false">J399-159000</f>
-        <v>654200</v>
-      </c>
+      <c r="H399" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I399" s="2"/>
+      <c r="J399" s="2"/>
+      <c r="K399" s="6" t="n">
+        <f aca="false">K397-K398</f>
+        <v>125000</v>
+      </c>
+      <c r="L399" s="4"/>
     </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L1048576" s="7" t="s">
@@ -10100,7 +10096,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="123">
+  <mergeCells count="127">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A24:C24"/>
@@ -10221,9 +10217,13 @@
     <mergeCell ref="A376:C376"/>
     <mergeCell ref="H376:J376"/>
     <mergeCell ref="A379:E379"/>
+    <mergeCell ref="H379:L379"/>
     <mergeCell ref="A397:C397"/>
+    <mergeCell ref="H397:J397"/>
     <mergeCell ref="A398:C398"/>
+    <mergeCell ref="H398:J398"/>
     <mergeCell ref="A399:C399"/>
+    <mergeCell ref="H399:J399"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10266,7 +10266,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="11" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="0" t="s">
@@ -10281,17 +10281,17 @@
       <c r="K2" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="P2" s="26"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>7685</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>16500</v>
@@ -10303,13 +10303,13 @@
         <v>27200</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>82200</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="K3" s="11" t="n">
         <v>42500</v>
@@ -10317,13 +10317,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>10458</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E4" s="11" t="n">
         <v>28470</v>
@@ -10340,14 +10340,14 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="27" t="s">
-        <v>281</v>
+      <c r="B5" s="26" t="s">
+        <v>270</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>20500</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E5" s="11" t="n">
         <v>24600</v>
@@ -10361,7 +10361,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>12500</v>
@@ -10377,7 +10377,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>13500</v>
@@ -10393,7 +10393,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>53200</v>
@@ -10409,7 +10409,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>39400</v>
@@ -10450,7 +10450,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="28"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="n">
         <f aca="false">(E10-E5)/2</f>
@@ -10481,12 +10481,12 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
+      <c r="A13" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -10500,12 +10500,12 @@
         <v>1</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" s="30" t="n">
+        <v>277</v>
+      </c>
+      <c r="C14" s="29" t="n">
         <v>360000</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -10519,12 +10519,12 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C15" s="30" t="n">
+        <v>278</v>
+      </c>
+      <c r="C15" s="29" t="n">
         <v>135000</v>
       </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -10538,12 +10538,12 @@
         <v>3</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="C16" s="30" t="n">
+        <v>279</v>
+      </c>
+      <c r="C16" s="29" t="n">
         <v>190000</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -10557,12 +10557,12 @@
         <v>4</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="C17" s="30" t="n">
+        <v>280</v>
+      </c>
+      <c r="C17" s="29" t="n">
         <v>5000</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -10576,12 +10576,12 @@
         <v>5</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="C18" s="30" t="n">
+        <v>281</v>
+      </c>
+      <c r="C18" s="29" t="n">
         <v>30000</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="29"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -10595,12 +10595,12 @@
         <v>6</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="C19" s="30" t="n">
+        <v>282</v>
+      </c>
+      <c r="C19" s="29" t="n">
         <v>90000</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="29"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -10614,12 +10614,12 @@
         <v>7</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="C20" s="30" t="n">
+        <v>283</v>
+      </c>
+      <c r="C20" s="29" t="n">
         <v>35000</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="29"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -10633,12 +10633,12 @@
         <v>8</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C21" s="30" t="n">
+        <v>284</v>
+      </c>
+      <c r="C21" s="29" t="n">
         <v>900000</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -10650,13 +10650,13 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" s="30" t="n">
+        <v>285</v>
+      </c>
+      <c r="C22" s="29" t="n">
         <f aca="false">SUM(C14:C21)</f>
         <v>1745000</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -10668,8 +10668,8 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -10679,18 +10679,18 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>300</v>
+      <c r="A24" s="30"/>
+      <c r="B24" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>289</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -10704,15 +10704,15 @@
         <v>1</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="C25" s="30" t="n">
+        <v>290</v>
+      </c>
+      <c r="C25" s="29" t="n">
         <v>600000</v>
       </c>
-      <c r="D25" s="30" t="n">
+      <c r="D25" s="29" t="n">
         <v>600000</v>
       </c>
-      <c r="E25" s="30" t="n">
+      <c r="E25" s="29" t="n">
         <f aca="false">C25-D25</f>
         <v>0</v>
       </c>
@@ -10728,15 +10728,15 @@
         <v>2</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="C26" s="30" t="n">
+        <v>291</v>
+      </c>
+      <c r="C26" s="29" t="n">
         <v>300000</v>
       </c>
-      <c r="D26" s="30" t="n">
+      <c r="D26" s="29" t="n">
         <v>300000</v>
       </c>
-      <c r="E26" s="30" t="n">
+      <c r="E26" s="29" t="n">
         <f aca="false">C26-D26</f>
         <v>0</v>
       </c>
@@ -10752,15 +10752,15 @@
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="C27" s="30" t="n">
+        <v>292</v>
+      </c>
+      <c r="C27" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D27" s="30" t="n">
+      <c r="D27" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E27" s="30" t="n">
+      <c r="E27" s="29" t="n">
         <f aca="false">C27-D27</f>
         <v>0</v>
       </c>
@@ -10778,13 +10778,13 @@
       <c r="B28" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="C28" s="30" t="n">
+      <c r="C28" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D28" s="30" t="n">
+      <c r="D28" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E28" s="30" t="n">
+      <c r="E28" s="29" t="n">
         <f aca="false">C28-D28</f>
         <v>0</v>
       </c>
@@ -10802,13 +10802,13 @@
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="30" t="n">
+      <c r="C29" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D29" s="30" t="n">
+      <c r="D29" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E29" s="30" t="n">
+      <c r="E29" s="29" t="n">
         <f aca="false">C29-D29</f>
         <v>0</v>
       </c>
@@ -10826,13 +10826,13 @@
       <c r="B30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="30" t="n">
+      <c r="C30" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D30" s="30" t="n">
+      <c r="D30" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E30" s="30" t="n">
+      <c r="E30" s="29" t="n">
         <f aca="false">C30-D30</f>
         <v>0</v>
       </c>
@@ -10850,13 +10850,13 @@
       <c r="B31" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="C31" s="30" t="n">
+      <c r="C31" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D31" s="30" t="n">
+      <c r="D31" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E31" s="30" t="n">
+      <c r="E31" s="29" t="n">
         <f aca="false">C31-D31</f>
         <v>0</v>
       </c>
@@ -10872,15 +10872,15 @@
         <v>8</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="C32" s="30" t="n">
+        <v>293</v>
+      </c>
+      <c r="C32" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D32" s="30" t="n">
+      <c r="D32" s="29" t="n">
         <v>90000</v>
       </c>
-      <c r="E32" s="30" t="n">
+      <c r="E32" s="29" t="n">
         <f aca="false">C32-D32</f>
         <v>10000</v>
       </c>
@@ -10890,15 +10890,15 @@
         <v>9</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="C33" s="30" t="n">
+        <v>294</v>
+      </c>
+      <c r="C33" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D33" s="30" t="n">
+      <c r="D33" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E33" s="30" t="n">
+      <c r="E33" s="29" t="n">
         <f aca="false">C33-D33</f>
         <v>0</v>
       </c>
@@ -10908,15 +10908,15 @@
         <v>10</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="C34" s="30" t="n">
+        <v>295</v>
+      </c>
+      <c r="C34" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D34" s="30" t="n">
+      <c r="D34" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E34" s="30" t="n">
+      <c r="E34" s="29" t="n">
         <f aca="false">C34-D34</f>
         <v>0</v>
       </c>
@@ -10926,13 +10926,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="C35" s="30" t="n">
+        <v>296</v>
+      </c>
+      <c r="C35" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30" t="n">
+      <c r="D35" s="29"/>
+      <c r="E35" s="29" t="n">
         <f aca="false">C35-D35</f>
         <v>100000</v>
       </c>
@@ -10942,15 +10942,15 @@
         <v>12</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="C36" s="30" t="n">
+        <v>297</v>
+      </c>
+      <c r="C36" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="D36" s="30" t="n">
+      <c r="D36" s="29" t="n">
         <v>100000</v>
       </c>
-      <c r="E36" s="30" t="n">
+      <c r="E36" s="29" t="n">
         <f aca="false">C36-D36</f>
         <v>0</v>
       </c>
@@ -10962,11 +10962,11 @@
         <f aca="false">SUM(C25:C36)</f>
         <v>1900000</v>
       </c>
-      <c r="D37" s="30" t="n">
+      <c r="D37" s="29" t="n">
         <f aca="false">SUM(D25:D36)</f>
         <v>1790000</v>
       </c>
-      <c r="E37" s="30" t="n">
+      <c r="E37" s="29" t="n">
         <f aca="false">C37-D37</f>
         <v>110000</v>
       </c>

</xml_diff>

<commit_message>
modify quy and CV
</commit_message>
<xml_diff>
--- a/Quy Phong.xlsx
+++ b/Quy Phong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="298">
   <si>
     <t>Thang 01/2012</t>
   </si>
@@ -1309,7 +1309,7 @@
   <dimension ref="A5:Q65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F372" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I386" activeCellId="0" sqref="I386"/>
+      <selection pane="topLeft" activeCell="I388" activeCellId="0" sqref="I388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9859,10 +9859,16 @@
       <c r="H386" s="19" t="n">
         <v>7</v>
       </c>
-      <c r="I386" s="4"/>
+      <c r="I386" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="J386" s="4"/>
-      <c r="K386" s="4"/>
-      <c r="L386" s="4"/>
+      <c r="K386" s="4" t="n">
+        <v>32000</v>
+      </c>
+      <c r="L386" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="19" t="n">
@@ -9875,10 +9881,16 @@
       <c r="H387" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="I387" s="4"/>
+      <c r="I387" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="J387" s="24"/>
-      <c r="K387" s="4"/>
-      <c r="L387" s="4"/>
+      <c r="K387" s="4" t="n">
+        <v>43000</v>
+      </c>
+      <c r="L387" s="4" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="19" t="n">
@@ -10064,7 +10076,7 @@
       <c r="J398" s="2"/>
       <c r="K398" s="4" t="n">
         <f aca="false">SUMIF(I381:I396,"C",K381:K396)</f>
-        <v>4038000</v>
+        <v>4113000</v>
       </c>
       <c r="L398" s="4"/>
     </row>
@@ -10086,7 +10098,7 @@
       <c r="J399" s="2"/>
       <c r="K399" s="6" t="n">
         <f aca="false">K397-K398</f>
-        <v>125000</v>
+        <v>50000</v>
       </c>
       <c r="L399" s="4"/>
     </row>

</xml_diff>

<commit_message>
update Quy Phong NOV 2015
</commit_message>
<xml_diff>
--- a/Quy Phong.xlsx
+++ b/Quy Phong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="309">
   <si>
     <t>Thang 01/2012</t>
   </si>
@@ -808,10 +808,40 @@
     <t>Quy Thang 08/2015</t>
   </si>
   <si>
+    <t>Quy Thang 09/2015</t>
+  </si>
+  <si>
     <t>Tien sieu thi</t>
   </si>
   <si>
     <t>tien kiem phong tro</t>
+  </si>
+  <si>
+    <t>Quy Thang 10/2015</t>
+  </si>
+  <si>
+    <t>Trung dong tien nha</t>
+  </si>
+  <si>
+    <t>4 thang dong tien nha</t>
+  </si>
+  <si>
+    <t>coc tien nha</t>
+  </si>
+  <si>
+    <t>o khoa</t>
+  </si>
+  <si>
+    <t>cafe luc ky HD</t>
+  </si>
+  <si>
+    <t>dien nuoc nt cu</t>
+  </si>
+  <si>
+    <t>nuoc uong nt cu</t>
+  </si>
+  <si>
+    <t>nuoc uong nt moi</t>
   </si>
   <si>
     <t>lau</t>
@@ -1311,8 +1341,8 @@
   </sheetPr>
   <dimension ref="A5:Q65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F372" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I389" activeCellId="0" sqref="I389"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D396" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K410" activeCellId="0" sqref="K410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1332,7 +1362,7 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.2793522267206"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2834008097166"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9229,7 +9259,7 @@
       </c>
       <c r="L353" s="4"/>
     </row>
-    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="17" t="s">
         <v>258</v>
       </c>
@@ -9245,7 +9275,7 @@
       <c r="K356" s="17"/>
       <c r="L356" s="17"/>
     </row>
-    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="2" t="s">
         <v>2</v>
       </c>
@@ -9277,7 +9307,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="18" t="n">
         <v>1</v>
       </c>
@@ -9305,7 +9335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="18" t="n">
         <v>2</v>
       </c>
@@ -9335,7 +9365,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="18" t="n">
         <v>4</v>
       </c>
@@ -9363,7 +9393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="18" t="n">
         <v>5</v>
       </c>
@@ -9391,7 +9421,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="18" t="n">
         <v>6</v>
       </c>
@@ -9419,7 +9449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="19" t="n">
         <v>7</v>
       </c>
@@ -9441,7 +9471,7 @@
       <c r="K363" s="4"/>
       <c r="L363" s="4"/>
     </row>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="19" t="n">
         <v>8</v>
       </c>
@@ -9457,7 +9487,7 @@
       <c r="K364" s="4"/>
       <c r="L364" s="4"/>
     </row>
-    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="19" t="n">
         <v>9</v>
       </c>
@@ -9473,7 +9503,7 @@
       <c r="K365" s="4"/>
       <c r="L365" s="4"/>
     </row>
-    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="18" t="n">
         <v>10</v>
       </c>
@@ -9489,7 +9519,7 @@
       <c r="K366" s="4"/>
       <c r="L366" s="4"/>
     </row>
-    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="18" t="n">
         <v>11</v>
       </c>
@@ -9505,7 +9535,7 @@
       <c r="K367" s="4"/>
       <c r="L367" s="4"/>
     </row>
-    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="18" t="n">
         <v>12</v>
       </c>
@@ -9521,7 +9551,7 @@
       <c r="K368" s="4"/>
       <c r="L368" s="4"/>
     </row>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="18" t="n">
         <v>13</v>
       </c>
@@ -9537,7 +9567,7 @@
       <c r="K369" s="4"/>
       <c r="L369" s="4"/>
     </row>
-    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="18" t="n">
         <v>26</v>
       </c>
@@ -9553,7 +9583,7 @@
       <c r="K370" s="4"/>
       <c r="L370" s="4"/>
     </row>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="18" t="n">
         <v>27</v>
       </c>
@@ -9569,7 +9599,7 @@
       <c r="K371" s="4"/>
       <c r="L371" s="4"/>
     </row>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="18" t="n">
         <v>28</v>
       </c>
@@ -9585,7 +9615,7 @@
       <c r="K372" s="4"/>
       <c r="L372" s="4"/>
     </row>
-    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="18" t="n">
         <v>29</v>
       </c>
@@ -9601,7 +9631,7 @@
       <c r="K373" s="4"/>
       <c r="L373" s="4"/>
     </row>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="2" t="s">
         <v>36</v>
       </c>
@@ -9623,7 +9653,7 @@
       </c>
       <c r="L374" s="4"/>
     </row>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="2" t="s">
         <v>37</v>
       </c>
@@ -9645,7 +9675,7 @@
       </c>
       <c r="L375" s="4"/>
     </row>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="2" t="s">
         <v>38</v>
       </c>
@@ -9667,7 +9697,7 @@
       </c>
       <c r="L376" s="4"/>
     </row>
-    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="17" t="s">
         <v>261</v>
       </c>
@@ -9676,14 +9706,14 @@
       <c r="D379" s="17"/>
       <c r="E379" s="17"/>
       <c r="H379" s="17" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="I379" s="17"/>
       <c r="J379" s="17"/>
       <c r="K379" s="17"/>
       <c r="L379" s="17"/>
     </row>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2" t="s">
         <v>2</v>
       </c>
@@ -9715,7 +9745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="18" t="n">
         <v>1</v>
       </c>
@@ -9743,7 +9773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="18" t="n">
         <v>2</v>
       </c>
@@ -9773,7 +9803,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="18" t="n">
         <v>4</v>
       </c>
@@ -9801,7 +9831,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="18" t="n">
         <v>5</v>
       </c>
@@ -9813,7 +9843,7 @@
         <v>307000</v>
       </c>
       <c r="E384" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H384" s="18" t="n">
         <v>5</v>
@@ -9826,10 +9856,10 @@
         <v>104000</v>
       </c>
       <c r="L384" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="18" t="n">
         <v>6</v>
       </c>
@@ -9851,7 +9881,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="19" t="n">
         <v>7</v>
       </c>
@@ -9873,7 +9903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="19" t="n">
         <v>8</v>
       </c>
@@ -9895,7 +9925,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="19" t="n">
         <v>9</v>
       </c>
@@ -9914,10 +9944,10 @@
         <v>200000</v>
       </c>
       <c r="L388" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="18" t="n">
         <v>10</v>
       </c>
@@ -9933,7 +9963,7 @@
       <c r="K389" s="4"/>
       <c r="L389" s="4"/>
     </row>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="18" t="n">
         <v>11</v>
       </c>
@@ -9949,7 +9979,7 @@
       <c r="K390" s="4"/>
       <c r="L390" s="4"/>
     </row>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="18" t="n">
         <v>12</v>
       </c>
@@ -9965,7 +9995,7 @@
       <c r="K391" s="4"/>
       <c r="L391" s="4"/>
     </row>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="18" t="n">
         <v>13</v>
       </c>
@@ -9981,7 +10011,7 @@
       <c r="K392" s="4"/>
       <c r="L392" s="4"/>
     </row>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="18" t="n">
         <v>26</v>
       </c>
@@ -9997,7 +10027,7 @@
       <c r="K393" s="4"/>
       <c r="L393" s="4"/>
     </row>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="18" t="n">
         <v>27</v>
       </c>
@@ -10013,7 +10043,7 @@
       <c r="K394" s="4"/>
       <c r="L394" s="4"/>
     </row>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="18" t="n">
         <v>28</v>
       </c>
@@ -10029,7 +10059,7 @@
       <c r="K395" s="4"/>
       <c r="L395" s="4"/>
     </row>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="18" t="n">
         <v>29</v>
       </c>
@@ -10045,7 +10075,7 @@
       <c r="K396" s="4"/>
       <c r="L396" s="4"/>
     </row>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="2" t="s">
         <v>36</v>
       </c>
@@ -10067,7 +10097,7 @@
       </c>
       <c r="L397" s="4"/>
     </row>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="2" t="s">
         <v>37</v>
       </c>
@@ -10089,7 +10119,7 @@
       </c>
       <c r="L398" s="4"/>
     </row>
-    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="2" t="s">
         <v>38</v>
       </c>
@@ -10111,13 +10141,449 @@
       </c>
       <c r="L399" s="4"/>
     </row>
+    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B402" s="17"/>
+      <c r="C402" s="17"/>
+      <c r="D402" s="17"/>
+      <c r="E402" s="17"/>
+      <c r="H402" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="I402" s="17"/>
+      <c r="J402" s="17"/>
+      <c r="K402" s="17"/>
+      <c r="L402" s="17"/>
+    </row>
+    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E403" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H403" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I403" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J403" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K403" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L403" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B404" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C404" s="23"/>
+      <c r="D404" s="4" t="n">
+        <v>-150000</v>
+      </c>
+      <c r="E404" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H404" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I404" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J404" s="23"/>
+      <c r="K404" s="4" t="n">
+        <v>-2454000</v>
+      </c>
+      <c r="L404" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B405" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C405" s="23"/>
+      <c r="D405" s="4" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="E405" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="H405" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I405" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J405" s="23"/>
+      <c r="K405" s="4" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="L405" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B406" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C406" s="23"/>
+      <c r="D406" s="4" t="n">
+        <v>3500000</v>
+      </c>
+      <c r="E406" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H406" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I406" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J406" s="23"/>
+      <c r="K406" s="4" t="n">
+        <v>130000</v>
+      </c>
+      <c r="L406" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B407" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C407" s="4"/>
+      <c r="D407" s="4" t="n">
+        <v>30000</v>
+      </c>
+      <c r="E407" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="H407" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="I407" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J407" s="4"/>
+      <c r="K407" s="4" t="n">
+        <v>80000</v>
+      </c>
+      <c r="L407" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B408" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C408" s="23"/>
+      <c r="D408" s="4" t="n">
+        <v>774000</v>
+      </c>
+      <c r="E408" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="H408" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="I408" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J408" s="23"/>
+      <c r="K408" s="4" t="n">
+        <v>16000</v>
+      </c>
+      <c r="L408" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="B409" s="4"/>
+      <c r="C409" s="4"/>
+      <c r="D409" s="4"/>
+      <c r="E409" s="4"/>
+      <c r="H409" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I409" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J409" s="4"/>
+      <c r="K409" s="4" t="n">
+        <v>34000</v>
+      </c>
+      <c r="L409" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="B410" s="4"/>
+      <c r="C410" s="24"/>
+      <c r="D410" s="4"/>
+      <c r="E410" s="4"/>
+      <c r="H410" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="I410" s="4"/>
+      <c r="J410" s="24"/>
+      <c r="K410" s="4"/>
+      <c r="L410" s="4"/>
+    </row>
+    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B411" s="4"/>
+      <c r="C411" s="24"/>
+      <c r="D411" s="4"/>
+      <c r="E411" s="4"/>
+      <c r="H411" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="I411" s="4"/>
+      <c r="J411" s="24"/>
+      <c r="K411" s="4"/>
+      <c r="L411" s="4"/>
+    </row>
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B412" s="4"/>
+      <c r="C412" s="23"/>
+      <c r="D412" s="4"/>
+      <c r="E412" s="4"/>
+      <c r="H412" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I412" s="4"/>
+      <c r="J412" s="23"/>
+      <c r="K412" s="4"/>
+      <c r="L412" s="4"/>
+    </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="B413" s="4"/>
+      <c r="C413" s="23"/>
+      <c r="D413" s="4"/>
+      <c r="E413" s="4"/>
+      <c r="H413" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="I413" s="4"/>
+      <c r="J413" s="23"/>
+      <c r="K413" s="4"/>
+      <c r="L413" s="4"/>
+    </row>
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="B414" s="4"/>
+      <c r="C414" s="23"/>
+      <c r="D414" s="4"/>
+      <c r="E414" s="4"/>
+      <c r="H414" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="I414" s="4"/>
+      <c r="J414" s="23"/>
+      <c r="K414" s="4"/>
+      <c r="L414" s="4"/>
+    </row>
+    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="B415" s="4"/>
+      <c r="C415" s="23"/>
+      <c r="D415" s="4"/>
+      <c r="E415" s="4"/>
+      <c r="H415" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="I415" s="4"/>
+      <c r="J415" s="23"/>
+      <c r="K415" s="4"/>
+      <c r="L415" s="4"/>
+    </row>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="B416" s="4"/>
+      <c r="C416" s="23"/>
+      <c r="D416" s="4"/>
+      <c r="E416" s="4"/>
+      <c r="H416" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="I416" s="4"/>
+      <c r="J416" s="23"/>
+      <c r="K416" s="4"/>
+      <c r="L416" s="4"/>
+    </row>
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="B417" s="4"/>
+      <c r="C417" s="23"/>
+      <c r="D417" s="4"/>
+      <c r="E417" s="4"/>
+      <c r="H417" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="I417" s="4"/>
+      <c r="J417" s="23"/>
+      <c r="K417" s="4"/>
+      <c r="L417" s="4"/>
+    </row>
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="B418" s="4"/>
+      <c r="C418" s="23"/>
+      <c r="D418" s="4"/>
+      <c r="E418" s="4"/>
+      <c r="H418" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="I418" s="4"/>
+      <c r="J418" s="23"/>
+      <c r="K418" s="4"/>
+      <c r="L418" s="4"/>
+    </row>
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="B419" s="4"/>
+      <c r="C419" s="23"/>
+      <c r="D419" s="4"/>
+      <c r="E419" s="4"/>
+      <c r="H419" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="I419" s="4"/>
+      <c r="J419" s="23"/>
+      <c r="K419" s="4"/>
+      <c r="L419" s="4"/>
+    </row>
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B420" s="2"/>
+      <c r="C420" s="2"/>
+      <c r="D420" s="4" t="n">
+        <f aca="false">SUMIF(B404:B419,"T",D404:D419)</f>
+        <v>1850000</v>
+      </c>
+      <c r="E420" s="4"/>
+      <c r="H420" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I420" s="2"/>
+      <c r="J420" s="2"/>
+      <c r="K420" s="4" t="n">
+        <f aca="false">SUMIF(I404:I419,"T",K404:K419)</f>
+        <v>5546000</v>
+      </c>
+      <c r="L420" s="4"/>
+    </row>
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B421" s="2"/>
+      <c r="C421" s="2"/>
+      <c r="D421" s="4" t="n">
+        <f aca="false">SUMIF(B404:B419,"C",D404:D419)</f>
+        <v>4304000</v>
+      </c>
+      <c r="E421" s="4"/>
+      <c r="H421" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I421" s="2"/>
+      <c r="J421" s="2"/>
+      <c r="K421" s="4" t="n">
+        <f aca="false">SUMIF(I404:I419,"C",K404:K419)</f>
+        <v>260000</v>
+      </c>
+      <c r="L421" s="4"/>
+    </row>
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B422" s="2"/>
+      <c r="C422" s="2"/>
+      <c r="D422" s="6" t="n">
+        <f aca="false">D420-D421</f>
+        <v>-2454000</v>
+      </c>
+      <c r="E422" s="4"/>
+      <c r="H422" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I422" s="2"/>
+      <c r="J422" s="2"/>
+      <c r="K422" s="6" t="n">
+        <f aca="false">K420-K421</f>
+        <v>5286000</v>
+      </c>
+      <c r="L422" s="4"/>
+    </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L1048576" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="127">
+  <mergeCells count="135">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A24:C24"/>
@@ -10245,10 +10711,18 @@
     <mergeCell ref="H398:J398"/>
     <mergeCell ref="A399:C399"/>
     <mergeCell ref="H399:J399"/>
+    <mergeCell ref="A402:E402"/>
+    <mergeCell ref="H402:L402"/>
+    <mergeCell ref="A420:C420"/>
+    <mergeCell ref="H420:J420"/>
+    <mergeCell ref="A421:C421"/>
+    <mergeCell ref="H421:J421"/>
+    <mergeCell ref="A422:C422"/>
+    <mergeCell ref="H422:J422"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -10269,7 +10743,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5708502024291"/>
@@ -10278,16 +10752,16 @@
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9959514170041"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.99595141700405"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="11" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="0" t="s">
@@ -10306,13 +10780,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>7685</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>16500</v>
@@ -10324,13 +10798,13 @@
         <v>27200</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>82200</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="K3" s="11" t="n">
         <v>42500</v>
@@ -10338,13 +10812,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>10458</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="E4" s="11" t="n">
         <v>28470</v>
@@ -10362,13 +10836,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="26" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>20500</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="E5" s="11" t="n">
         <v>24600</v>
@@ -10382,7 +10856,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>12500</v>
@@ -10398,7 +10872,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>13500</v>
@@ -10414,7 +10888,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>53200</v>
@@ -10430,7 +10904,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>39400</v>
@@ -10503,7 +10977,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -10521,7 +10995,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C14" s="29" t="n">
         <v>360000</v>
@@ -10540,7 +11014,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="C15" s="29" t="n">
         <v>135000</v>
@@ -10559,7 +11033,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="C16" s="29" t="n">
         <v>190000</v>
@@ -10578,7 +11052,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="C17" s="29" t="n">
         <v>5000</v>
@@ -10597,7 +11071,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="C18" s="29" t="n">
         <v>30000</v>
@@ -10616,7 +11090,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="C19" s="29" t="n">
         <v>90000</v>
@@ -10635,7 +11109,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="C20" s="29" t="n">
         <v>35000</v>
@@ -10654,7 +11128,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="C21" s="29" t="n">
         <v>900000</v>
@@ -10671,7 +11145,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="18" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="C22" s="29" t="n">
         <f aca="false">SUM(C14:C21)</f>
@@ -10702,16 +11176,16 @@
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="30"/>
       <c r="B24" s="31" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="E24" s="32" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -10725,7 +11199,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="C25" s="29" t="n">
         <v>600000</v>
@@ -10749,7 +11223,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="C26" s="29" t="n">
         <v>300000</v>
@@ -10773,7 +11247,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C27" s="29" t="n">
         <v>100000</v>
@@ -10893,7 +11367,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="C32" s="29" t="n">
         <v>100000</v>
@@ -10911,7 +11385,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="C33" s="29" t="n">
         <v>100000</v>
@@ -10929,7 +11403,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="C34" s="29" t="n">
         <v>100000</v>
@@ -10947,7 +11421,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C35" s="29" t="n">
         <v>100000</v>
@@ -10963,7 +11437,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C36" s="29" t="n">
         <v>100000</v>
@@ -11003,7 +11477,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -11024,7 +11498,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
update quy phong thang 01/2016
</commit_message>
<xml_diff>
--- a/Quy Phong.xlsx
+++ b/Quy Phong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="318">
   <si>
     <t>Thang 01/2012</t>
   </si>
@@ -820,6 +820,9 @@
     <t>Quy Thang 10/2015</t>
   </si>
   <si>
+    <t>Quy Thang 11/2015</t>
+  </si>
+  <si>
     <t>Trung dong tien nha</t>
   </si>
   <si>
@@ -842,6 +845,30 @@
   </si>
   <si>
     <t>nuoc uong nt moi</t>
+  </si>
+  <si>
+    <t>tien phong T11+12</t>
+  </si>
+  <si>
+    <t>Quy Thang 12/2015</t>
+  </si>
+  <si>
+    <t>Quy Thang 1/2016</t>
+  </si>
+  <si>
+    <t>nc xa + choi</t>
+  </si>
+  <si>
+    <t>dong tien nha thang 1</t>
+  </si>
+  <si>
+    <t>xa don</t>
+  </si>
+  <si>
+    <t>nuoc xit phong</t>
+  </si>
+  <si>
+    <t>nuoc rua tay</t>
   </si>
   <si>
     <t>lau</t>
@@ -1063,7 +1090,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1083,6 +1110,13 @@
       <right/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1113,7 +1147,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1211,6 +1245,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1341,8 +1383,8 @@
   </sheetPr>
   <dimension ref="A5:Q65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D396" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K410" activeCellId="0" sqref="K410"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C415" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H426" activeCellId="0" sqref="H426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1362,7 +1404,7 @@
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.2793522267206"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2834008097166"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10141,7 +10183,7 @@
       </c>
       <c r="L399" s="4"/>
     </row>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="17" t="s">
         <v>265</v>
       </c>
@@ -10150,14 +10192,14 @@
       <c r="D402" s="17"/>
       <c r="E402" s="17"/>
       <c r="H402" s="17" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I402" s="17"/>
       <c r="J402" s="17"/>
       <c r="K402" s="17"/>
       <c r="L402" s="17"/>
     </row>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="2" t="s">
         <v>2</v>
       </c>
@@ -10189,7 +10231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="18" t="n">
         <v>1</v>
       </c>
@@ -10217,7 +10259,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="18" t="n">
         <v>2</v>
       </c>
@@ -10229,7 +10271,7 @@
         <v>2000000</v>
       </c>
       <c r="E405" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H405" s="18" t="n">
         <v>2</v>
@@ -10242,10 +10284,10 @@
         <v>8000000</v>
       </c>
       <c r="L405" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="18" t="n">
         <v>4</v>
       </c>
@@ -10257,7 +10299,7 @@
         <v>3500000</v>
       </c>
       <c r="E406" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H406" s="18" t="n">
         <v>4</v>
@@ -10270,10 +10312,10 @@
         <v>130000</v>
       </c>
       <c r="L406" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="18" t="n">
         <v>5</v>
       </c>
@@ -10285,7 +10327,7 @@
         <v>30000</v>
       </c>
       <c r="E407" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H407" s="18" t="n">
         <v>5</v>
@@ -10301,7 +10343,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="18" t="n">
         <v>6</v>
       </c>
@@ -10313,7 +10355,7 @@
         <v>774000</v>
       </c>
       <c r="E408" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="H408" s="18" t="n">
         <v>6</v>
@@ -10326,10 +10368,10 @@
         <v>16000</v>
       </c>
       <c r="L408" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="19" t="n">
         <v>7</v>
       </c>
@@ -10348,10 +10390,10 @@
         <v>34000</v>
       </c>
       <c r="L409" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="19" t="n">
         <v>8</v>
       </c>
@@ -10362,12 +10404,18 @@
       <c r="H410" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="I410" s="4"/>
+      <c r="I410" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="J410" s="24"/>
-      <c r="K410" s="4"/>
-      <c r="L410" s="4"/>
-    </row>
-    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K410" s="4" t="n">
+        <v>5016000</v>
+      </c>
+      <c r="L410" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="19" t="n">
         <v>9</v>
       </c>
@@ -10383,7 +10431,7 @@
       <c r="K411" s="4"/>
       <c r="L411" s="4"/>
     </row>
-    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="18" t="n">
         <v>10</v>
       </c>
@@ -10399,7 +10447,7 @@
       <c r="K412" s="4"/>
       <c r="L412" s="4"/>
     </row>
-    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="18" t="n">
         <v>11</v>
       </c>
@@ -10415,7 +10463,7 @@
       <c r="K413" s="4"/>
       <c r="L413" s="4"/>
     </row>
-    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="18" t="n">
         <v>12</v>
       </c>
@@ -10431,7 +10479,7 @@
       <c r="K414" s="4"/>
       <c r="L414" s="4"/>
     </row>
-    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="18" t="n">
         <v>13</v>
       </c>
@@ -10447,7 +10495,7 @@
       <c r="K415" s="4"/>
       <c r="L415" s="4"/>
     </row>
-    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="18" t="n">
         <v>26</v>
       </c>
@@ -10463,7 +10511,7 @@
       <c r="K416" s="4"/>
       <c r="L416" s="4"/>
     </row>
-    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="18" t="n">
         <v>27</v>
       </c>
@@ -10479,7 +10527,7 @@
       <c r="K417" s="4"/>
       <c r="L417" s="4"/>
     </row>
-    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="18" t="n">
         <v>28</v>
       </c>
@@ -10495,7 +10543,7 @@
       <c r="K418" s="4"/>
       <c r="L418" s="4"/>
     </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="18" t="n">
         <v>29</v>
       </c>
@@ -10511,7 +10559,7 @@
       <c r="K419" s="4"/>
       <c r="L419" s="4"/>
     </row>
-    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="2" t="s">
         <v>36</v>
       </c>
@@ -10533,7 +10581,7 @@
       </c>
       <c r="L420" s="4"/>
     </row>
-    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="2" t="s">
         <v>37</v>
       </c>
@@ -10551,11 +10599,11 @@
       <c r="J421" s="2"/>
       <c r="K421" s="4" t="n">
         <f aca="false">SUMIF(I404:I419,"C",K404:K419)</f>
-        <v>260000</v>
+        <v>5276000</v>
       </c>
       <c r="L421" s="4"/>
     </row>
-    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="2" t="s">
         <v>38</v>
       </c>
@@ -10573,17 +10621,474 @@
       <c r="J422" s="2"/>
       <c r="K422" s="6" t="n">
         <f aca="false">K420-K421</f>
-        <v>5286000</v>
+        <v>270000</v>
       </c>
       <c r="L422" s="4"/>
     </row>
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="B425" s="17"/>
+      <c r="C425" s="17"/>
+      <c r="D425" s="17"/>
+      <c r="E425" s="17"/>
+      <c r="H425" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="I425" s="17"/>
+      <c r="J425" s="17"/>
+      <c r="K425" s="17"/>
+      <c r="L425" s="17"/>
+    </row>
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B426" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D426" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E426" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H426" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I426" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J426" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K426" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L426" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B427" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C427" s="23"/>
+      <c r="D427" s="4" t="n">
+        <v>270000</v>
+      </c>
+      <c r="E427" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H427" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I427" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J427" s="23"/>
+      <c r="K427" s="4" t="n">
+        <v>211000</v>
+      </c>
+      <c r="L427" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B428" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C428" s="23"/>
+      <c r="D428" s="4" t="n">
+        <f aca="false">1200000*5</f>
+        <v>6000000</v>
+      </c>
+      <c r="E428" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H428" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I428" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J428" s="23"/>
+      <c r="K428" s="4" t="n">
+        <f aca="false">1000000*5</f>
+        <v>5000000</v>
+      </c>
+      <c r="L428" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B429" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C429" s="23"/>
+      <c r="D429" s="4" t="n">
+        <v>100000</v>
+      </c>
+      <c r="E429" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="H429" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I429" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J429" s="23"/>
+      <c r="K429" s="4" t="n">
+        <v>4900000</v>
+      </c>
+      <c r="L429" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B430" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C430" s="4"/>
+      <c r="D430" s="4" t="n">
+        <v>310000</v>
+      </c>
+      <c r="E430" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="H430" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="I430" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J430" s="4"/>
+      <c r="K430" s="4" t="n">
+        <v>34000</v>
+      </c>
+      <c r="L430" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B431" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C431" s="23"/>
+      <c r="D431" s="4" t="n">
+        <v>5500000</v>
+      </c>
+      <c r="E431" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="H431" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="I431" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J431" s="23"/>
+      <c r="K431" s="4" t="n">
+        <v>35000</v>
+      </c>
+      <c r="L431" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="B432" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C432" s="4"/>
+      <c r="D432" s="4" t="n">
+        <v>90000</v>
+      </c>
+      <c r="E432" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H432" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="I432" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J432" s="4"/>
+      <c r="K432" s="25"/>
+      <c r="L432" s="25"/>
+    </row>
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="B433" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C433" s="24"/>
+      <c r="D433" s="4" t="n">
+        <v>34000</v>
+      </c>
+      <c r="E433" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H433" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="I433" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J433" s="24"/>
+      <c r="K433" s="25"/>
+      <c r="L433" s="25"/>
+    </row>
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B434" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C434" s="24"/>
+      <c r="D434" s="4" t="n">
+        <v>25000</v>
+      </c>
+      <c r="E434" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="H434" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="I434" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J434" s="24"/>
+      <c r="K434" s="25"/>
+      <c r="L434" s="25"/>
+    </row>
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B435" s="4"/>
+      <c r="C435" s="23"/>
+      <c r="D435" s="4"/>
+      <c r="E435" s="4"/>
+      <c r="H435" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I435" s="4"/>
+      <c r="J435" s="23"/>
+      <c r="K435" s="26"/>
+      <c r="L435" s="26"/>
+    </row>
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="B436" s="4"/>
+      <c r="C436" s="23"/>
+      <c r="D436" s="4"/>
+      <c r="E436" s="4"/>
+      <c r="H436" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="I436" s="4"/>
+      <c r="J436" s="23"/>
+      <c r="K436" s="4"/>
+      <c r="L436" s="4"/>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="B437" s="4"/>
+      <c r="C437" s="23"/>
+      <c r="D437" s="4"/>
+      <c r="E437" s="4"/>
+      <c r="H437" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="I437" s="4"/>
+      <c r="J437" s="23"/>
+      <c r="K437" s="4"/>
+      <c r="L437" s="4"/>
+    </row>
+    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="B438" s="4"/>
+      <c r="C438" s="23"/>
+      <c r="D438" s="4"/>
+      <c r="E438" s="4"/>
+      <c r="H438" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="I438" s="4"/>
+      <c r="J438" s="23"/>
+      <c r="K438" s="4"/>
+      <c r="L438" s="4"/>
+    </row>
+    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="B439" s="4"/>
+      <c r="C439" s="23"/>
+      <c r="D439" s="4"/>
+      <c r="E439" s="4"/>
+      <c r="H439" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="I439" s="4"/>
+      <c r="J439" s="23"/>
+      <c r="K439" s="4"/>
+      <c r="L439" s="4"/>
+    </row>
+    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="B440" s="4"/>
+      <c r="C440" s="23"/>
+      <c r="D440" s="4"/>
+      <c r="E440" s="4"/>
+      <c r="H440" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="I440" s="4"/>
+      <c r="J440" s="23"/>
+      <c r="K440" s="4"/>
+      <c r="L440" s="4"/>
+    </row>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="B441" s="4"/>
+      <c r="C441" s="23"/>
+      <c r="D441" s="4"/>
+      <c r="E441" s="4"/>
+      <c r="H441" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="I441" s="4"/>
+      <c r="J441" s="23"/>
+      <c r="K441" s="4"/>
+      <c r="L441" s="4"/>
+    </row>
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="B442" s="4"/>
+      <c r="C442" s="23"/>
+      <c r="D442" s="4"/>
+      <c r="E442" s="4"/>
+      <c r="H442" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="I442" s="4"/>
+      <c r="J442" s="23"/>
+      <c r="K442" s="4"/>
+      <c r="L442" s="4"/>
+    </row>
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B443" s="2"/>
+      <c r="C443" s="2"/>
+      <c r="D443" s="4" t="n">
+        <f aca="false">SUMIF(B427:B442,"T",D427:D442)</f>
+        <v>6270000</v>
+      </c>
+      <c r="E443" s="4"/>
+      <c r="H443" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I443" s="2"/>
+      <c r="J443" s="2"/>
+      <c r="K443" s="4" t="n">
+        <f aca="false">SUMIF(I427:I442,"T",K427:K442)</f>
+        <v>5211000</v>
+      </c>
+      <c r="L443" s="4"/>
+    </row>
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B444" s="2"/>
+      <c r="C444" s="2"/>
+      <c r="D444" s="4" t="n">
+        <f aca="false">SUMIF(B427:B442,"C",D427:D442)</f>
+        <v>6059000</v>
+      </c>
+      <c r="E444" s="4"/>
+      <c r="H444" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I444" s="2"/>
+      <c r="J444" s="2"/>
+      <c r="K444" s="4" t="n">
+        <f aca="false">SUMIF(I427:I442,"C",K427:K442)</f>
+        <v>4969000</v>
+      </c>
+      <c r="L444" s="4"/>
+    </row>
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B445" s="2"/>
+      <c r="C445" s="2"/>
+      <c r="D445" s="6" t="n">
+        <f aca="false">D443-D444</f>
+        <v>211000</v>
+      </c>
+      <c r="E445" s="4"/>
+      <c r="H445" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I445" s="2"/>
+      <c r="J445" s="2"/>
+      <c r="K445" s="6" t="n">
+        <f aca="false">K443-K444</f>
+        <v>242000</v>
+      </c>
+      <c r="L445" s="4"/>
+    </row>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L1048576" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="135">
+  <mergeCells count="143">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A24:C24"/>
@@ -10719,6 +11224,14 @@
     <mergeCell ref="H421:J421"/>
     <mergeCell ref="A422:C422"/>
     <mergeCell ref="H422:J422"/>
+    <mergeCell ref="A425:E425"/>
+    <mergeCell ref="H425:L425"/>
+    <mergeCell ref="A443:C443"/>
+    <mergeCell ref="H443:J443"/>
+    <mergeCell ref="A444:C444"/>
+    <mergeCell ref="H444:J444"/>
+    <mergeCell ref="A445:C445"/>
+    <mergeCell ref="H445:J445"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -10761,7 +11274,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="11" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="0" t="s">
@@ -10776,17 +11289,17 @@
       <c r="K2" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="P2" s="25"/>
+      <c r="P2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>7685</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>16500</v>
@@ -10798,13 +11311,13 @@
         <v>27200</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>82200</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="K3" s="11" t="n">
         <v>42500</v>
@@ -10812,13 +11325,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>10458</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="E4" s="11" t="n">
         <v>28470</v>
@@ -10835,14 +11348,14 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="26" t="s">
-        <v>281</v>
+      <c r="B5" s="28" t="s">
+        <v>290</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>20500</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="E5" s="11" t="n">
         <v>24600</v>
@@ -10856,7 +11369,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>12500</v>
@@ -10872,7 +11385,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>13500</v>
@@ -10888,7 +11401,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>53200</v>
@@ -10904,7 +11417,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>39400</v>
@@ -10945,7 +11458,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="27"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="n">
         <f aca="false">(E10-E5)/2</f>
@@ -10976,12 +11489,12 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="s">
-        <v>287</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="A13" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -10995,12 +11508,12 @@
         <v>1</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" s="29" t="n">
+        <v>297</v>
+      </c>
+      <c r="C14" s="31" t="n">
         <v>360000</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -11014,12 +11527,12 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C15" s="29" t="n">
+        <v>298</v>
+      </c>
+      <c r="C15" s="31" t="n">
         <v>135000</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
@@ -11033,12 +11546,12 @@
         <v>3</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="C16" s="29" t="n">
+        <v>299</v>
+      </c>
+      <c r="C16" s="31" t="n">
         <v>190000</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="31"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -11052,12 +11565,12 @@
         <v>4</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="C17" s="29" t="n">
+        <v>300</v>
+      </c>
+      <c r="C17" s="31" t="n">
         <v>5000</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -11071,12 +11584,12 @@
         <v>5</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="C18" s="29" t="n">
+        <v>301</v>
+      </c>
+      <c r="C18" s="31" t="n">
         <v>30000</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -11090,12 +11603,12 @@
         <v>6</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="C19" s="29" t="n">
+        <v>302</v>
+      </c>
+      <c r="C19" s="31" t="n">
         <v>90000</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
@@ -11109,12 +11622,12 @@
         <v>7</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="C20" s="29" t="n">
+        <v>303</v>
+      </c>
+      <c r="C20" s="31" t="n">
         <v>35000</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -11128,12 +11641,12 @@
         <v>8</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C21" s="29" t="n">
+        <v>304</v>
+      </c>
+      <c r="C21" s="31" t="n">
         <v>900000</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -11145,13 +11658,13 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" s="29" t="n">
+        <v>305</v>
+      </c>
+      <c r="C22" s="31" t="n">
         <f aca="false">SUM(C14:C21)</f>
         <v>1745000</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -11163,8 +11676,8 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -11174,18 +11687,18 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>298</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>300</v>
+      <c r="A24" s="32"/>
+      <c r="B24" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>309</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -11199,15 +11712,15 @@
         <v>1</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="C25" s="29" t="n">
+        <v>310</v>
+      </c>
+      <c r="C25" s="31" t="n">
         <v>600000</v>
       </c>
-      <c r="D25" s="29" t="n">
+      <c r="D25" s="31" t="n">
         <v>600000</v>
       </c>
-      <c r="E25" s="29" t="n">
+      <c r="E25" s="31" t="n">
         <f aca="false">C25-D25</f>
         <v>0</v>
       </c>
@@ -11223,15 +11736,15 @@
         <v>2</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="C26" s="29" t="n">
+        <v>311</v>
+      </c>
+      <c r="C26" s="31" t="n">
         <v>300000</v>
       </c>
-      <c r="D26" s="29" t="n">
+      <c r="D26" s="31" t="n">
         <v>300000</v>
       </c>
-      <c r="E26" s="29" t="n">
+      <c r="E26" s="31" t="n">
         <f aca="false">C26-D26</f>
         <v>0</v>
       </c>
@@ -11247,15 +11760,15 @@
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="C27" s="29" t="n">
+        <v>312</v>
+      </c>
+      <c r="C27" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D27" s="29" t="n">
+      <c r="D27" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E27" s="29" t="n">
+      <c r="E27" s="31" t="n">
         <f aca="false">C27-D27</f>
         <v>0</v>
       </c>
@@ -11273,13 +11786,13 @@
       <c r="B28" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="C28" s="29" t="n">
+      <c r="C28" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D28" s="29" t="n">
+      <c r="D28" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E28" s="29" t="n">
+      <c r="E28" s="31" t="n">
         <f aca="false">C28-D28</f>
         <v>0</v>
       </c>
@@ -11297,13 +11810,13 @@
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="29" t="n">
+      <c r="C29" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D29" s="29" t="n">
+      <c r="D29" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E29" s="29" t="n">
+      <c r="E29" s="31" t="n">
         <f aca="false">C29-D29</f>
         <v>0</v>
       </c>
@@ -11321,13 +11834,13 @@
       <c r="B30" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="29" t="n">
+      <c r="C30" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D30" s="29" t="n">
+      <c r="D30" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E30" s="29" t="n">
+      <c r="E30" s="31" t="n">
         <f aca="false">C30-D30</f>
         <v>0</v>
       </c>
@@ -11345,13 +11858,13 @@
       <c r="B31" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="C31" s="29" t="n">
+      <c r="C31" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D31" s="29" t="n">
+      <c r="D31" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E31" s="29" t="n">
+      <c r="E31" s="31" t="n">
         <f aca="false">C31-D31</f>
         <v>0</v>
       </c>
@@ -11367,15 +11880,15 @@
         <v>8</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="C32" s="29" t="n">
+        <v>313</v>
+      </c>
+      <c r="C32" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D32" s="29" t="n">
+      <c r="D32" s="31" t="n">
         <v>90000</v>
       </c>
-      <c r="E32" s="29" t="n">
+      <c r="E32" s="31" t="n">
         <f aca="false">C32-D32</f>
         <v>10000</v>
       </c>
@@ -11385,15 +11898,15 @@
         <v>9</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="C33" s="29" t="n">
+        <v>314</v>
+      </c>
+      <c r="C33" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D33" s="29" t="n">
+      <c r="D33" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E33" s="29" t="n">
+      <c r="E33" s="31" t="n">
         <f aca="false">C33-D33</f>
         <v>0</v>
       </c>
@@ -11403,15 +11916,15 @@
         <v>10</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="C34" s="29" t="n">
+        <v>315</v>
+      </c>
+      <c r="C34" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D34" s="29" t="n">
+      <c r="D34" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E34" s="29" t="n">
+      <c r="E34" s="31" t="n">
         <f aca="false">C34-D34</f>
         <v>0</v>
       </c>
@@ -11421,13 +11934,13 @@
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>307</v>
-      </c>
-      <c r="C35" s="29" t="n">
+        <v>316</v>
+      </c>
+      <c r="C35" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29" t="n">
+      <c r="D35" s="31"/>
+      <c r="E35" s="31" t="n">
         <f aca="false">C35-D35</f>
         <v>100000</v>
       </c>
@@ -11437,15 +11950,15 @@
         <v>12</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="C36" s="29" t="n">
+        <v>317</v>
+      </c>
+      <c r="C36" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="D36" s="29" t="n">
+      <c r="D36" s="31" t="n">
         <v>100000</v>
       </c>
-      <c r="E36" s="29" t="n">
+      <c r="E36" s="31" t="n">
         <f aca="false">C36-D36</f>
         <v>0</v>
       </c>
@@ -11457,11 +11970,11 @@
         <f aca="false">SUM(C25:C36)</f>
         <v>1900000</v>
       </c>
-      <c r="D37" s="29" t="n">
+      <c r="D37" s="31" t="n">
         <f aca="false">SUM(D25:D36)</f>
         <v>1790000</v>
       </c>
-      <c r="E37" s="29" t="n">
+      <c r="E37" s="31" t="n">
         <f aca="false">C37-D37</f>
         <v>110000</v>
       </c>

</xml_diff>

<commit_message>
update room fund on april
</commit_message>
<xml_diff>
--- a/Quy Phong.xlsx
+++ b/Quy Phong.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="323">
   <si>
     <t>Thang 01/2012</t>
   </si>
@@ -874,10 +874,16 @@
     <t>Quy Thang 2/2016</t>
   </si>
   <si>
+    <t>Quy Thang 3/2016</t>
+  </si>
+  <si>
     <t>dong tien nha thang 2</t>
   </si>
   <si>
     <t>tay bon cau</t>
+  </si>
+  <si>
+    <t>Quy Thang 4/2016</t>
   </si>
   <si>
     <t>lau</t>
@@ -1306,22 +1312,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1392,8 +1382,8 @@
   </sheetPr>
   <dimension ref="A5:Q65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E442" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I455" activeCellId="0" sqref="I455"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A463" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H480" activeCellId="0" sqref="H480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11100,7 +11090,7 @@
       <c r="D448" s="17"/>
       <c r="E448" s="17"/>
       <c r="H448" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I448" s="17"/>
       <c r="J448" s="17"/>
@@ -11208,7 +11198,7 @@
         <v>4340000</v>
       </c>
       <c r="E452" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="H452" s="18" t="n">
         <v>4</v>
@@ -11338,7 +11328,7 @@
         <v>33700</v>
       </c>
       <c r="E457" s="25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H457" s="19" t="n">
         <v>9</v>
@@ -11542,13 +11532,250 @@
       </c>
       <c r="L468" s="4"/>
     </row>
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B470" s="17"/>
+      <c r="C470" s="17"/>
+      <c r="D470" s="17"/>
+      <c r="E470" s="17"/>
+    </row>
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C471" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D471" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E471" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B472" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C472" s="23"/>
+      <c r="D472" s="4" t="n">
+        <v>736000</v>
+      </c>
+      <c r="E472" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B473" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C473" s="23"/>
+      <c r="D473" s="4" t="n">
+        <f aca="false">1350000*4</f>
+        <v>5400000</v>
+      </c>
+      <c r="E473" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B474" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C474" s="23"/>
+      <c r="D474" s="4" t="n">
+        <v>5355000</v>
+      </c>
+      <c r="E474" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B475" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C475" s="4"/>
+      <c r="D475" s="4" t="n">
+        <v>80000</v>
+      </c>
+      <c r="E475" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="B476" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C476" s="23"/>
+      <c r="D476" s="4" t="n">
+        <v>34000</v>
+      </c>
+      <c r="E476" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="19" t="n">
+        <v>7</v>
+      </c>
+      <c r="B477" s="4"/>
+      <c r="C477" s="4"/>
+      <c r="D477" s="4"/>
+      <c r="E477" s="25"/>
+    </row>
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="19" t="n">
+        <v>8</v>
+      </c>
+      <c r="B478" s="4"/>
+      <c r="C478" s="24"/>
+      <c r="D478" s="4"/>
+      <c r="E478" s="25"/>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="19" t="n">
+        <v>9</v>
+      </c>
+      <c r="B479" s="4"/>
+      <c r="C479" s="24"/>
+      <c r="D479" s="4"/>
+      <c r="E479" s="25"/>
+    </row>
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="B480" s="4"/>
+      <c r="C480" s="23"/>
+      <c r="D480" s="26"/>
+      <c r="E480" s="26"/>
+    </row>
+    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="B481" s="4"/>
+      <c r="C481" s="23"/>
+      <c r="D481" s="4"/>
+      <c r="E481" s="4"/>
+    </row>
+    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="B482" s="4"/>
+      <c r="C482" s="23"/>
+      <c r="D482" s="4"/>
+      <c r="E482" s="4"/>
+    </row>
+    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="18" t="n">
+        <v>13</v>
+      </c>
+      <c r="B483" s="4"/>
+      <c r="C483" s="23"/>
+      <c r="D483" s="4"/>
+      <c r="E483" s="4"/>
+    </row>
+    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="18" t="n">
+        <v>26</v>
+      </c>
+      <c r="B484" s="4"/>
+      <c r="C484" s="23"/>
+      <c r="D484" s="4"/>
+      <c r="E484" s="4"/>
+    </row>
+    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="18" t="n">
+        <v>27</v>
+      </c>
+      <c r="B485" s="4"/>
+      <c r="C485" s="23"/>
+      <c r="D485" s="4"/>
+      <c r="E485" s="4"/>
+    </row>
+    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="18" t="n">
+        <v>28</v>
+      </c>
+      <c r="B486" s="4"/>
+      <c r="C486" s="23"/>
+      <c r="D486" s="4"/>
+      <c r="E486" s="4"/>
+    </row>
+    <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="18" t="n">
+        <v>29</v>
+      </c>
+      <c r="B487" s="4"/>
+      <c r="C487" s="23"/>
+      <c r="D487" s="4"/>
+      <c r="E487" s="4"/>
+    </row>
+    <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B488" s="2"/>
+      <c r="C488" s="2"/>
+      <c r="D488" s="4" t="n">
+        <f aca="false">SUMIF(B472:B487,"T",D472:D487)</f>
+        <v>6136000</v>
+      </c>
+      <c r="E488" s="4"/>
+    </row>
+    <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B489" s="2"/>
+      <c r="C489" s="2"/>
+      <c r="D489" s="4" t="n">
+        <f aca="false">SUMIF(B472:B487,"C",D472:D487)</f>
+        <v>5469000</v>
+      </c>
+      <c r="E489" s="4"/>
+    </row>
+    <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B490" s="2"/>
+      <c r="C490" s="2"/>
+      <c r="D490" s="6" t="n">
+        <f aca="false">D488-D489</f>
+        <v>667000</v>
+      </c>
+      <c r="E490" s="4"/>
+    </row>
     <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L1048576" s="7" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="151">
+  <mergeCells count="155">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A24:C24"/>
@@ -11700,6 +11927,10 @@
     <mergeCell ref="H467:J467"/>
     <mergeCell ref="A468:C468"/>
     <mergeCell ref="H468:J468"/>
+    <mergeCell ref="A470:E470"/>
+    <mergeCell ref="A488:C488"/>
+    <mergeCell ref="A489:C489"/>
+    <mergeCell ref="A490:C490"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -11742,7 +11973,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="11" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="0" t="s">
@@ -11761,13 +11992,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C3" s="11" t="n">
         <v>7685</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E3" s="11" t="n">
         <v>16500</v>
@@ -11779,13 +12010,13 @@
         <v>27200</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="I3" s="11" t="n">
         <v>82200</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="K3" s="11" t="n">
         <v>42500</v>
@@ -11793,13 +12024,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>10458</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="E4" s="11" t="n">
         <v>28470</v>
@@ -11817,13 +12048,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="28" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C5" s="11" t="n">
         <v>20500</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E5" s="11" t="n">
         <v>24600</v>
@@ -11837,7 +12068,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C6" s="11" t="n">
         <v>12500</v>
@@ -11853,7 +12084,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C7" s="11" t="n">
         <v>13500</v>
@@ -11869,7 +12100,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>53200</v>
@@ -11885,7 +12116,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C9" s="11" t="n">
         <v>39400</v>
@@ -11958,7 +12189,7 @@
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="30" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -11976,7 +12207,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C14" s="31" t="n">
         <v>360000</v>
@@ -11995,7 +12226,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C15" s="31" t="n">
         <v>135000</v>
@@ -12014,7 +12245,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C16" s="31" t="n">
         <v>190000</v>
@@ -12033,7 +12264,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C17" s="31" t="n">
         <v>5000</v>
@@ -12052,7 +12283,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C18" s="31" t="n">
         <v>30000</v>
@@ -12071,7 +12302,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C19" s="31" t="n">
         <v>90000</v>
@@ -12090,7 +12321,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C20" s="31" t="n">
         <v>35000</v>
@@ -12109,7 +12340,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C21" s="31" t="n">
         <v>900000</v>
@@ -12126,7 +12357,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="18" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C22" s="31" t="n">
         <f aca="false">SUM(C14:C21)</f>
@@ -12157,16 +12388,16 @@
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="32"/>
       <c r="B24" s="33" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -12180,7 +12411,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C25" s="31" t="n">
         <v>600000</v>
@@ -12204,7 +12435,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C26" s="31" t="n">
         <v>300000</v>
@@ -12228,7 +12459,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C27" s="31" t="n">
         <v>100000</v>
@@ -12348,7 +12579,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C32" s="31" t="n">
         <v>100000</v>
@@ -12366,7 +12597,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C33" s="31" t="n">
         <v>100000</v>
@@ -12384,7 +12615,7 @@
         <v>10</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C34" s="31" t="n">
         <v>100000</v>
@@ -12402,7 +12633,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C35" s="31" t="n">
         <v>100000</v>
@@ -12418,7 +12649,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C36" s="31" t="n">
         <v>100000</v>

</xml_diff>